<commit_message>
Private Email doen not work to this program. Company email is neccessary with authentication
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\UiPathProjects\InventoryAlert_UiPath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DD9908-3DF4-43D9-9EBB-34F2A43F7E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE53CB1-2504-44F1-B1E5-BBC9656AF7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -611,7 +611,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>80</v>

</xml_diff>